<commit_message>
Edit Database Migration and model
</commit_message>
<xml_diff>
--- a/documents/DACNTT2.1.xlsx
+++ b/documents/DACNTT2.1.xlsx
@@ -79,13 +79,7 @@
     <t>Thiết kế hệ thống</t>
   </si>
   <si>
-    <t>Vẽ Class Diagram</t>
-  </si>
-  <si>
     <t>Phân tích và thiết kế cơ sở dữ liệu; Chọn 1 DBMS để thiết kế cơ sở dữ liệu; Chạy demo</t>
-  </si>
-  <si>
-    <t>Vẽ mô hình ERD dưới gốc nhìn vật lý của hệ thống; tạo và viết migration trong laravel; chạy migration trong laravel; export code SQL từ phpMyAdmin</t>
   </si>
   <si>
     <t>Ghi chú</t>
@@ -97,12 +91,20 @@
     <t>Chọn công nghệ cho back-end.</t>
   </si>
   <si>
-    <t>Tìm hiểu VueJS.
+    <t>Tìm hiểu Laravel
 Khó khăn: chưa có tài liệu hay ví dụ cụ thể về cách đăng nhập và phân quyền cho việc kết hợp Laravel và VueJS lại với nhau.</t>
   </si>
   <si>
-    <t>Tìm hiểu Laravel
-Khó khăn: chưa có tài liệu hay ví dụ cụ thể về cách đăng nhập và phân quyền cho việc kết hợp Laravel và VueJS lại với nhau.</t>
+    <t>Tạo và viết migration trong laravel; chạy migration trong laravel.
+Export code SQL từ phpMyAdmin.</t>
+  </si>
+  <si>
+    <t>Vẽ ER Diagram; Vẽ Class Diagram</t>
+  </si>
+  <si>
+    <t>Tìm hiểu VueJS.
+Khó khăn: chưa có tài liệu hay ví dụ cụ thể về cách đăng nhập và phân quyền cho việc kết hợp Laravel và VueJS lại với nhau.
+Chọn Blade template</t>
   </si>
 </sst>
 </file>
@@ -479,8 +481,8 @@
   </sheetPr>
   <dimension ref="A1:AD985"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -724,7 +726,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>12</v>
@@ -815,7 +817,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="19">
@@ -845,7 +847,7 @@
       <c r="AC9" s="2"/>
       <c r="AD9" s="2"/>
     </row>
-    <row r="10" spans="1:30" ht="75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="15">
         <v>3</v>
       </c>
@@ -858,14 +860,14 @@
         <v>44137</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="19">
-        <v>0.73</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -891,7 +893,7 @@
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
     </row>
-    <row r="11" spans="1:30" ht="75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" ht="90" x14ac:dyDescent="0.2">
       <c r="A11" s="15">
         <v>4</v>
       </c>
@@ -904,11 +906,11 @@
         <v>44144</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G11" s="19">
         <v>0</v>
@@ -950,11 +952,11 @@
         <v>44151</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G12" s="19">
         <v>0</v>

</xml_diff>

<commit_message>
SQL and documents updates
</commit_message>
<xml_diff>
--- a/documents/DACNTT2.1.xlsx
+++ b/documents/DACNTT2.1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN DỰ ÁN CÔNG NGHỆ THÔNG TIN 2</t>
   </si>
@@ -119,6 +119,12 @@
     <t>Xây dựng chức năng quản lý khoa.
 Xây dựng chức năng quản lý lớp.
 Xây dựng chức năng quản lý thông tin giảng viên</t>
+  </si>
+  <si>
+    <t>Thiết kế cơ sở dữ liệu cho chức năng quản lý môn học</t>
+  </si>
+  <si>
+    <t>Thiết kế cơ sở dữ liệu cho chức năng quản lý điểm.</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <dimension ref="A1:AE985"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1029,13 +1035,15 @@
       <c r="D13" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="18"/>
+      <c r="E13" s="18" t="s">
+        <v>31</v>
+      </c>
       <c r="F13" s="18" t="s">
         <v>27</v>
       </c>
       <c r="G13" s="18"/>
       <c r="H13" s="19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1076,13 +1084,15 @@
       <c r="D14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="18"/>
+      <c r="E14" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="F14" s="18" t="s">
         <v>28</v>
       </c>
       <c r="G14" s="18"/>
       <c r="H14" s="19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>

</xml_diff>